<commit_message>
tightened up ncalc vs n, and Gcalc vs G
</commit_message>
<xml_diff>
--- a/Engineering/Requirements/untitled folder/Phase_4_OET_65_Worksheet.xlsx
+++ b/Engineering/Requirements/untitled folder/Phase_4_OET_65_Worksheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Maximum power density at the surface</t>
   </si>
@@ -95,15 +95,9 @@
     <t>W/(m*m)</t>
   </si>
   <si>
-    <t>calculated aperture efficiency</t>
-  </si>
-  <si>
     <t>ncalc</t>
   </si>
   <si>
-    <t>power gain in direction of interest relative to isotropic radiator</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>decimal</t>
   </si>
   <si>
-    <t>calculated power gain in direction of interest relative to isotropic radiator</t>
-  </si>
-  <si>
     <t>Gcalc</t>
   </si>
   <si>
@@ -152,7 +143,28 @@
     <t>dB</t>
   </si>
   <si>
-    <t>calculated power gain in direction of interest relative to isotropic radiator (dB)</t>
+    <t>estimated power gain in direction of interest relative to isotropic radiator</t>
+  </si>
+  <si>
+    <t>estimated power gain in direction of interest relative to isotropic radiator (dB)</t>
+  </si>
+  <si>
+    <t>GcalcdB</t>
+  </si>
+  <si>
+    <t>calculated aperture efficiency using estimated Gain G</t>
+  </si>
+  <si>
+    <t>calculated power gain in direction of interest relative to isotropic radiator using estimated n</t>
+  </si>
+  <si>
+    <t>calculated power gain in direction of interest relative to isotropic radiator using estimated n (dB)</t>
+  </si>
+  <si>
+    <t>if you now the efficiency n, then you can calculate the gain Gcalc</t>
+  </si>
+  <si>
+    <t>if  you know the Gain G, then you can calculate efficiency ncalc</t>
   </si>
 </sst>
 </file>
@@ -484,15 +496,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.33203125" customWidth="1"/>
+    <col min="1" max="1" width="84.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -520,7 +532,7 @@
       </c>
       <c r="C2" s="1">
         <f>(4*C3)/C4</f>
-        <v>3.4217671183422809</v>
+        <v>25.150410760200742</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>22</v>
@@ -549,7 +561,7 @@
       </c>
       <c r="C4">
         <f>PI()*(C6/2)*(C6/2)</f>
-        <v>1.168986626400762</v>
+        <v>0.15904312808798329</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -564,7 +576,7 @@
       </c>
       <c r="C5" s="1">
         <f>((C6*C6)/(4*C7))</f>
-        <v>7.0202866666666663</v>
+        <v>0.955125</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -578,37 +590,37 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1.22</v>
+        <v>0.45</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
-        <f>C16/C15</f>
+      <c r="C7" s="1">
+        <f>C17/C16</f>
         <v>5.3003533568904596E-2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="1">
         <f>(16*C9*C3)/(PI()*C6*C6)</f>
-        <v>1.7108835591711404</v>
+        <v>12.575205380100371</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -623,104 +635,133 @@
         <v>0.5</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1">
         <f>(16*C11*C3)/(PI()*C6*C6)</f>
-        <v>0</v>
+        <v>14.141319933321556</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="C11" s="1">
         <f>((C12*C7*C7)/(4*PI())/((PI()*C6*C6/(4))))</f>
-        <v>0</v>
+        <v>0.5622699393721029</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>400</v>
+      </c>
+      <c r="D12" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1">
+        <f>10*LOG10(C12)</f>
+        <v>26.020599913279625</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1">
         <f>((4*PI()*C4*C9)/(C7*C7))</f>
-        <v>2614.4465290099415</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="3">
-        <v>27</v>
-      </c>
-      <c r="D14" s="3" t="s">
+        <v>355.7010360954805</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="3">
-        <v>5660000000</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>36</v>
+      <c r="C15" s="1">
+        <f>10*LOG10(C14)</f>
+        <v>25.510851302121917</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3">
+        <v>5660000000</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="3">
         <f>3*10^8</f>
         <v>300000000</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>39</v>
+      <c r="D17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>